<commit_message>
added setting prostate and start change business logic
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,10 +427,10 @@
     <col width="40" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
@@ -441,6 +441,10 @@
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -543,15 +547,38 @@
 (ширина)</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Предстательная железа
+(ширина)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Предстательная железа
+(высота)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Предстательная железа
+(передне-задний размер)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>объем железы</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Токтомушев К.</t>
+          <t>Боромбаева А. Т.</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1959</v>
+        <v>1962</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -560,12 +587,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>115х45</t>
+          <t>112х41</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>113х47</t>
+          <t>109х46</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -579,32 +606,44 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" t="n">
         <v>16</v>
       </c>
       <c r="N2" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O2" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P2" t="n">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q2" t="n">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="R2" t="n">
+        <v>52</v>
+      </c>
+      <c r="S2" t="n">
+        <v>33</v>
+      </c>
+      <c r="T2" t="n">
+        <v>42</v>
+      </c>
+      <c r="U2" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Боромбаева А. Т.</t>
+          <t>Апылова К.</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1962</v>
+        <v>1979</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -613,12 +652,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>112х41</t>
+          <t>97х36</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>109х46</t>
+          <t>91х39</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -631,33 +670,39 @@
           <t>не расширена</t>
         </is>
       </c>
-      <c r="L3" t="n">
-        <v>15</v>
-      </c>
-      <c r="M3" t="n">
-        <v>16</v>
-      </c>
       <c r="N3" t="n">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="O3" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P3" t="n">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="Q3" t="n">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="R3" t="n">
+        <v>44</v>
+      </c>
+      <c r="S3" t="n">
+        <v>24</v>
+      </c>
+      <c r="T3" t="n">
+        <v>38</v>
+      </c>
+      <c r="U3" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Айткул уулу Ильяс</t>
+          <t>Кожекова У.</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1987</v>
+        <v>1983</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -666,12 +711,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>115х45</t>
+          <t>114х42</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>118х51</t>
+          <t>109х47</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -685,32 +730,44 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O4" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P4" t="n">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="Q4" t="n">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="R4" t="n">
+        <v>49</v>
+      </c>
+      <c r="S4" t="n">
+        <v>24</v>
+      </c>
+      <c r="T4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U4" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Жумакешов С.</t>
+          <t>Тагаева Р.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1984</v>
+        <v>1970</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -719,12 +776,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>112х45</t>
+          <t>117х42</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>112х49</t>
+          <t>125х42</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -734,36 +791,36 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>не расширена</t>
-        </is>
+          <t>расширена</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>30</v>
       </c>
       <c r="L5" t="n">
-        <v>16</v>
-      </c>
-      <c r="M5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="O5" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P5" t="n">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="Q5" t="n">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Кожекова У.</t>
+          <t>Кокоев Ш.</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1983</v>
+        <v>2008</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -772,12 +829,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>114х42</t>
+          <t>98х37</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>109х47</t>
+          <t>102х35</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -787,36 +844,54 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>не расширена</t>
-        </is>
+          <t>расширена</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>27</v>
+      </c>
+      <c r="J6" t="n">
+        <v>11</v>
       </c>
       <c r="L6" t="n">
+        <v>12</v>
+      </c>
+      <c r="M6" t="n">
+        <v>12</v>
+      </c>
+      <c r="N6" t="n">
+        <v>98</v>
+      </c>
+      <c r="O6" t="n">
+        <v>37</v>
+      </c>
+      <c r="P6" t="n">
+        <v>102</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>35</v>
+      </c>
+      <c r="R6" t="n">
+        <v>41</v>
+      </c>
+      <c r="S6" t="n">
+        <v>21</v>
+      </c>
+      <c r="T6" t="n">
+        <v>36</v>
+      </c>
+      <c r="U6" t="n">
         <v>16</v>
-      </c>
-      <c r="M6" t="n">
-        <v>16</v>
-      </c>
-      <c r="N6" t="n">
-        <v>114</v>
-      </c>
-      <c r="O6" t="n">
-        <v>42</v>
-      </c>
-      <c r="P6" t="n">
-        <v>109</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Тагаева Р.</t>
+          <t>Рысмамбетов А.</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1970</v>
+        <v>1956</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -825,12 +900,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>117х42</t>
+          <t>104х41</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>125х42</t>
+          <t>110х44</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -840,36 +915,36 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>расширена</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>30</v>
+          <t>не расширена</t>
+        </is>
       </c>
       <c r="L7" t="n">
         <v>15</v>
       </c>
+      <c r="M7" t="n">
+        <v>15</v>
+      </c>
       <c r="N7" t="n">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="O7" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7" t="n">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="Q7" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ашимов Кубат</t>
+          <t>Эшкожоева А.</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1997</v>
+        <v>1974</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -878,51 +953,57 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>110х48</t>
+          <t>108х45</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>112х43</t>
+          <t>123х45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>не расширена</t>
+          <t>расширена</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>16</v>
-      </c>
-      <c r="M8" t="n">
-        <v>16</v>
+          <t>расширена</t>
+        </is>
       </c>
       <c r="N8" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O8" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="P8" t="n">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="Q8" t="n">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="R8" t="n">
+        <v>44</v>
+      </c>
+      <c r="S8" t="n">
+        <v>20</v>
+      </c>
+      <c r="T8" t="n">
+        <v>39</v>
+      </c>
+      <c r="U8" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кокоев Ш.</t>
+          <t>Убайдуллаева Н.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2008</v>
+        <v>1975</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -931,12 +1012,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>98х37</t>
+          <t>105х44</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>102х35</t>
+          <t>107х48</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -946,42 +1027,36 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>расширена</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>27</v>
-      </c>
-      <c r="J9" t="n">
-        <v>11</v>
+          <t>не расширена</t>
+        </is>
       </c>
       <c r="L9" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M9" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N9" t="n">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="O9" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="P9" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="Q9" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Рысмамбетов А.</t>
+          <t>Касымова К.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1956</v>
+        <v>2004</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -990,12 +1065,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>104х41</t>
+          <t>97х43</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>110х44</t>
+          <t>98х41</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1015,26 +1090,26 @@
         <v>15</v>
       </c>
       <c r="N10" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="O10" t="n">
+        <v>43</v>
+      </c>
+      <c r="P10" t="n">
+        <v>98</v>
+      </c>
+      <c r="Q10" t="n">
         <v>41</v>
-      </c>
-      <c r="P10" t="n">
-        <v>110</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кадиев С.</t>
+          <t>Турманбетов Кайрат</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1959</v>
+        <v>1997</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1043,12 +1118,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>101х43</t>
+          <t>102х40</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>105х44</t>
+          <t>110х45</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1060,6 +1135,9 @@
         <is>
           <t>не расширена</t>
         </is>
+      </c>
+      <c r="J11" t="n">
+        <v>4</v>
       </c>
       <c r="L11" t="n">
         <v>15</v>
@@ -1068,26 +1146,38 @@
         <v>15</v>
       </c>
       <c r="N11" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O11" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P11" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="Q11" t="n">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="R11" t="n">
+        <v>51</v>
+      </c>
+      <c r="S11" t="n">
+        <v>26</v>
+      </c>
+      <c r="T11" t="n">
+        <v>41</v>
+      </c>
+      <c r="U11" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Сарыбаев Э. Р.</t>
+          <t>Абдылдаев Максат</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1991</v>
+        <v>1982</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1096,12 +1186,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>121х45</t>
+          <t>112х46</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>120х48</t>
+          <t>116х49</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1121,26 +1211,26 @@
         <v>16</v>
       </c>
       <c r="N12" t="n">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="O12" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P12" t="n">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Q12" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Убайдуллаева Н.</t>
+          <t>Шабралиева С. Р.</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1975</v>
+        <v>1978</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1149,12 +1239,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>105х44</t>
+          <t>94х34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>107х48</t>
+          <t>93х38</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1168,32 +1258,44 @@
         </is>
       </c>
       <c r="L13" t="n">
+        <v>14</v>
+      </c>
+      <c r="M13" t="n">
+        <v>14</v>
+      </c>
+      <c r="N13" t="n">
+        <v>94</v>
+      </c>
+      <c r="O13" t="n">
+        <v>34</v>
+      </c>
+      <c r="P13" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>38</v>
+      </c>
+      <c r="R13" t="n">
+        <v>42</v>
+      </c>
+      <c r="S13" t="n">
+        <v>19</v>
+      </c>
+      <c r="T13" t="n">
+        <v>34</v>
+      </c>
+      <c r="U13" t="n">
         <v>15</v>
-      </c>
-      <c r="M13" t="n">
-        <v>15</v>
-      </c>
-      <c r="N13" t="n">
-        <v>105</v>
-      </c>
-      <c r="O13" t="n">
-        <v>44</v>
-      </c>
-      <c r="P13" t="n">
-        <v>107</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Касымова К.</t>
+          <t>Ишенбаев М.</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1202,12 +1304,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>97х43</t>
+          <t>107х43</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>98х41</t>
+          <t>102х38</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1227,26 +1329,38 @@
         <v>15</v>
       </c>
       <c r="N14" t="n">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="O14" t="n">
         <v>43</v>
       </c>
       <c r="P14" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="Q14" t="n">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="R14" t="n">
+        <v>44</v>
+      </c>
+      <c r="S14" t="n">
+        <v>24</v>
+      </c>
+      <c r="T14" t="n">
+        <v>36</v>
+      </c>
+      <c r="U14" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Койлубаев М.</t>
+          <t>Ашимбекова А.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1985</v>
+        <v>1999</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1255,17 +1369,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>110х46</t>
+          <t>131х54</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>114х45</t>
+          <t>121х49</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>не расширена</t>
+          <t>расширена</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1273,554 +1387,46 @@
           <t>не расширена</t>
         </is>
       </c>
-      <c r="L15" t="n">
-        <v>16</v>
-      </c>
-      <c r="M15" t="n">
-        <v>16</v>
+      <c r="H15" t="n">
+        <v>25</v>
       </c>
       <c r="N15" t="n">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="O15" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="P15" t="n">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="Q15" t="n">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="R15" t="n">
+        <v>49</v>
+      </c>
+      <c r="S15" t="n">
+        <v>20</v>
+      </c>
+      <c r="T15" t="n">
+        <v>42</v>
+      </c>
+      <c r="U15" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Турманбетов Кайрат</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>102х40</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>110х45</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>4</v>
-      </c>
-      <c r="L16" t="n">
-        <v>15</v>
-      </c>
-      <c r="M16" t="n">
-        <v>15</v>
-      </c>
-      <c r="N16" t="n">
-        <v>102</v>
-      </c>
-      <c r="O16" t="n">
-        <v>40</v>
-      </c>
-      <c r="P16" t="n">
-        <v>110</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Абдылдаев Максат</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1982</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>112х46</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>116х49</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>16</v>
-      </c>
-      <c r="M17" t="n">
-        <v>16</v>
-      </c>
-      <c r="N17" t="n">
-        <v>112</v>
-      </c>
-      <c r="O17" t="n">
-        <v>46</v>
-      </c>
-      <c r="P17" t="n">
-        <v>116</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Карымшаков Б.</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1996                                                                                                                                                   Дата исследования: 03.08.2021</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>105х44</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>104х47</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>16</v>
-      </c>
-      <c r="M18" t="n">
-        <v>16</v>
-      </c>
-      <c r="N18" t="n">
-        <v>105</v>
-      </c>
-      <c r="O18" t="n">
-        <v>44</v>
-      </c>
-      <c r="P18" t="n">
-        <v>104</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Шабралиева С. Р.</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1978</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>94х34</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>93х38</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L19" t="n">
-        <v>14</v>
-      </c>
-      <c r="M19" t="n">
-        <v>14</v>
-      </c>
-      <c r="N19" t="n">
-        <v>94</v>
-      </c>
-      <c r="O19" t="n">
-        <v>34</v>
-      </c>
-      <c r="P19" t="n">
-        <v>93</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Усубалиев Б.</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1990</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>105х45</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>107х45</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>15</v>
-      </c>
-      <c r="M20" t="n">
-        <v>15</v>
-      </c>
-      <c r="N20" t="n">
-        <v>105</v>
-      </c>
-      <c r="O20" t="n">
-        <v>45</v>
-      </c>
-      <c r="P20" t="n">
-        <v>107</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Wu Fei</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1984</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>106х42</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>106х51</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L21" t="n">
-        <v>16</v>
-      </c>
-      <c r="M21" t="n">
-        <v>16</v>
-      </c>
-      <c r="N21" t="n">
-        <v>106</v>
-      </c>
-      <c r="O21" t="n">
+      <c r="R16" t="n">
         <v>42</v>
       </c>
-      <c r="P21" t="n">
-        <v>106</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Ишенбаев М.</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>107х43</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>102х38</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L22" t="n">
-        <v>15</v>
-      </c>
-      <c r="M22" t="n">
-        <v>15</v>
-      </c>
-      <c r="N22" t="n">
-        <v>107</v>
-      </c>
-      <c r="O22" t="n">
-        <v>43</v>
-      </c>
-      <c r="P22" t="n">
-        <v>102</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Кенжегараев Б.</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1990</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>124х47</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>120х47</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L23" t="n">
-        <v>16</v>
-      </c>
-      <c r="M23" t="n">
-        <v>16</v>
-      </c>
-      <c r="N23" t="n">
-        <v>124</v>
-      </c>
-      <c r="O23" t="n">
-        <v>47</v>
-      </c>
-      <c r="P23" t="n">
-        <v>120</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Кыдыралиев К.</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1952</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>110х47</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>107х47</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>расширена</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>расширена</t>
-        </is>
-      </c>
-      <c r="L24" t="n">
-        <v>16</v>
-      </c>
-      <c r="M24" t="n">
-        <v>16</v>
-      </c>
-      <c r="N24" t="n">
-        <v>110</v>
-      </c>
-      <c r="O24" t="n">
-        <v>47</v>
-      </c>
-      <c r="P24" t="n">
-        <v>107</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="n">
-        <v>19</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>03.08.2021</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>122х61</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>122х61</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>не расширена</t>
-        </is>
-      </c>
-      <c r="L25" t="n">
-        <v>16</v>
-      </c>
-      <c r="M25" t="n">
-        <v>16</v>
-      </c>
-      <c r="N25" t="n">
-        <v>122</v>
-      </c>
-      <c r="O25" t="n">
-        <v>61</v>
-      </c>
-      <c r="P25" t="n">
-        <v>122</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>61</v>
+      <c r="S16" t="n">
+        <v>21</v>
+      </c>
+      <c r="T16" t="n">
+        <v>39</v>
+      </c>
+      <c r="U16" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>